<commit_message>
working tests. parses all cell types. multisheets
</commit_message>
<xml_diff>
--- a/test/spreadsheets/excel_mac_2008-formulas.xlsx
+++ b/test/spreadsheets/excel_mac_2008-formulas.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -19,9 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>bob</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bobfrompage2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -398,7 +403,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -419,8 +424,41 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="str">
+        <f>Sheet2!A1</f>
+        <v>bobfrompage2</v>
+      </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>